<commit_message>
Minor improvements to the text
</commit_message>
<xml_diff>
--- a/analysis_code/genomics/culture_MAGs_intermediate/Chx-S19-short-contamination-check.xlsx
+++ b/analysis_code/genomics/culture_MAGs_intermediate/Chx-S19-short-contamination-check.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmtsuji/Documents/Git/Ca-Chlorohelix-allophototropha-RCI/analysis_code/genomics/culture_MAGs_intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D212719-A46D-0544-9566-EAE9DE916E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4815970C-40A3-2A41-8C83-169507F758F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="1000" windowWidth="27900" windowHeight="15240" xr2:uid="{EA38CCFF-50F5-664E-B478-5F32AACDAB59}"/>
   </bookViews>
   <sheets>
     <sheet name="non-Chx-Geo-reads-S19.9-short" sheetId="1" r:id="rId1"/>
-    <sheet name="summary" sheetId="2" r:id="rId2"/>
+    <sheet name="summary_stats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>JACAUB010000010.1</t>
   </si>
@@ -207,55 +207,62 @@
     <t>合計 / reads</t>
   </si>
   <si>
-    <t>reads not on possible contaminant contigs from Chx</t>
+    <t>Contigs outside the Chlorohelix genome that had mapped reads from the Chx S19.9 short read metagenome</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>percent of total reads in Cfx3-03</t>
+    <t>mapped reads</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>possible contaminant reads in Cfx3-03 (%)</t>
+    <t>Did not have a close match to the Chlorohelix genome</t>
+  </si>
+  <si>
+    <t>Note: all contigs here have a close (&gt;=96.845% identity, 100% query coverage) match to the Chlorohelix L227-S17 genome unless indicated otherwise.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Contigs with &lt;100% identity to Chx (but still &gt;95% identity):</t>
+    <t>reads not on possible contaminant contigs from Chx (see first worksheet)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Test 1: reads with &gt;95% identity to Chx across 100% of sequence in Cfx3-03</t>
+    <t>All other reads appear to match Chlorohelix-like contigs.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Test 2: reads with 100% identity to Chx across 100% of sequence in Cfx3-03</t>
+    <t>Detailed check of reads mapping to the Cfx3-03 MAG:</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>All counts aside from these plus the 4 counts noted above have 100% identity across 100% of sequence to Chx</t>
+    <t>(These all still had &gt;95% identity to Chlorohelix)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Reads in Cfx3-03 with 100% identity across 100% of sequence to Chx</t>
+    <t>Contigs with &lt;99% identity to Chlorohelix that had mapped reads for Cfx3-03</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Percent of these reads among all reads mapping to Cfx3-03</t>
+    <t>All counts aside from these plus the 4 counts noted above are associated with contigs having &gt;99% identity across 100% of sequence to the Chlorohelix L227-S17 genome</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Test 2: reads with &gt;99% identity to Chx across 100% of sequence in Cfx3-03</t>
+    <t>Reads in Cfx3-03 that mapped to contigs having &gt;99% identity across 100% of sequence to Chlorohelix L227-S17</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Contigs with &lt;99% identity to Chx (but still &gt;95% identity):</t>
+    <t>count</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>All counts aside from these plus the 4 counts noted above have &gt;99% identity across 100% of sequence to Chx</t>
+    <t>% of all mapped reads to Cfx3-03</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Reads in Cfx3-03 with &gt;99% identity across 100% of sequence to Chx</t>
+    <t>Summary of reads mapping to non-Chlorohelix genomes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Overall, this is less than 2% of the total short reads from the S19.9 metagenome dataset (=6637225 total reads)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -263,7 +270,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="183" formatCode="0.0_ "/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -297,6 +307,13 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -326,7 +343,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -342,7 +359,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -365,7 +385,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Tsuji Jackson" refreshedDate="44966.919878587963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="44" xr:uid="{59720227-D572-5340-B941-7090FA44942A}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B1:C45" sheet="non-Chx-Geo-reads-S19.9-short"/>
+    <worksheetSource ref="B2:C46" sheet="non-Chx-Geo-reads-S19.9-short"/>
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="genome" numFmtId="0">
@@ -614,7 +634,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60771B2B-7363-A14F-8D7F-5317274A78EB}" name="ピボットテーブル1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60771B2B-7363-A14F-8D7F-5317274A78EB}" name="ピボットテーブル1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -1010,7 +1030,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97974083-3143-4349-B86C-2E25743C4146}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1019,499 +1039,514 @@
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3">
         <v>834</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
         <v>10212</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
         <v>2376</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
         <v>886</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
         <v>1115</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
         <v>2134</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
         <v>1530</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
         <v>860</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11">
         <v>758</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12">
         <v>609</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12">
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13">
         <v>1134</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
         <v>3312</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15">
         <v>808</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
         <v>2800</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16">
-        <v>989</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
       </c>
       <c r="C17">
-        <v>8782</v>
+        <v>989</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
         <v>44</v>
       </c>
       <c r="C18">
-        <v>1316</v>
+        <v>8782</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
       </c>
       <c r="C19">
-        <v>4679</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20">
-        <v>1607</v>
+        <v>4679</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>44</v>
       </c>
       <c r="C21">
-        <v>1582</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>44</v>
       </c>
       <c r="C22">
-        <v>20510</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
       <c r="C23">
-        <v>1407</v>
+        <v>20510</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>44</v>
       </c>
       <c r="C24">
-        <v>1563</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25">
-        <v>1865</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>44</v>
       </c>
       <c r="C26">
-        <v>2365</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
       </c>
       <c r="C27">
-        <v>1396</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
       </c>
       <c r="C28">
-        <v>3065</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
       <c r="C29">
-        <v>3317</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>44</v>
       </c>
       <c r="C30">
-        <v>645</v>
+        <v>3317</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
         <v>44</v>
       </c>
       <c r="C31">
-        <v>1017</v>
+        <v>645</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32">
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33">
         <v>1508</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33">
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34">
         <v>1087</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34">
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
         <v>3033</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35">
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36">
         <v>1670</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36">
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37">
         <v>833</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37">
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
         <v>21548</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39">
         <v>1106</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39">
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40">
         <v>4997</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40">
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41">
         <v>1110</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
       <c r="C42">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
       </c>
       <c r="C43">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+      <c r="D44" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>46</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>24</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>47</v>
       </c>
-      <c r="C45">
+      <c r="C46">
         <v>2</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1522,7 +1557,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C04C19-EE5F-5445-BCBE-875B4F59B2B4}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1534,7 +1569,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1548,7 +1583,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1558,12 +1593,8 @@
       <c r="B4">
         <v>122365</v>
       </c>
-      <c r="D4">
-        <f>D3/GETPIVOTDATA("reads",$A$3,"genome","Cfx3-03")*100</f>
-        <v>3.2689085931434641E-3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
+      <c r="D4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1573,13 +1604,6 @@
       <c r="B5">
         <v>1011</v>
       </c>
-      <c r="D5">
-        <f>100-D4</f>
-        <v>99.996731091406858</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
@@ -1604,15 +1628,18 @@
       <c r="B8">
         <v>123402</v>
       </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1628,207 +1655,91 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B14" t="str">
-        <f>VLOOKUP(A14,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
+        <f>VLOOKUP(A14,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,2,FALSE)</f>
         <v>Cfx3-03</v>
       </c>
       <c r="C14">
-        <f>VLOOKUP(A14,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>609</v>
+        <f>VLOOKUP(A14,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,3,FALSE)</f>
+        <v>989</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B15" t="str">
-        <f>VLOOKUP(A15,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
+        <f>VLOOKUP(A15,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,2,FALSE)</f>
         <v>Cfx3-03</v>
       </c>
       <c r="C15">
-        <f>VLOOKUP(A15,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>989</v>
+        <f>VLOOKUP(A15,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,3,FALSE)</f>
+        <v>1670</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" t="str">
-        <f>VLOOKUP(A16,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
+        <f>VLOOKUP(A16,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,2,FALSE)</f>
         <v>Cfx3-03</v>
       </c>
       <c r="C16">
-        <f>VLOOKUP(A16,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>1670</v>
+        <f>VLOOKUP(A16,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,3,FALSE)</f>
+        <v>833</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B17" t="str">
-        <f>VLOOKUP(A17,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
-        <v>Cfx3-03</v>
+        <f>VLOOKUP(A17,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,2,FALSE)</f>
+        <v>Cfx3-08</v>
       </c>
       <c r="C17">
-        <f>VLOOKUP(A17,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>833</v>
+        <f>VLOOKUP(A17,'non-Chx-Geo-reads-S19.9-short'!$A$2:$C$46,3,FALSE)</f>
+        <v>346</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="str">
-        <f>VLOOKUP(A18,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
-        <v>Cfx3-03</v>
-      </c>
-      <c r="C18">
-        <f>VLOOKUP(A18,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>4997</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="str">
-        <f>VLOOKUP(A19,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
-        <v>Cfx3-08</v>
-      </c>
       <c r="C19">
-        <f>VLOOKUP(A19,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>346</v>
+        <f>SUM(C14:C17)</f>
+        <v>3838</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="C21">
-        <f>SUM(C14:C19)</f>
-        <v>9444</v>
-      </c>
-      <c r="D21" t="s">
-        <v>60</v>
+      <c r="C21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22">
+        <f>GETPIVOTDATA("reads",$A$3,"genome","Cfx3-03")-C19</f>
+        <v>118527</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="C23">
-        <f>GETPIVOTDATA("reads",$A$3,"genome","Cfx3-03")-D3-C21</f>
-        <v>112917</v>
+      <c r="C23" s="6">
+        <f>C22/GETPIVOTDATA("reads",$A$3,"genome","Cfx3-03")*100</f>
+        <v>96.863482204878849</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="C24">
-        <f>C23/GETPIVOTDATA("reads",$A$3,"genome","Cfx3-03")*100</f>
-        <v>92.278837902995136</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="str">
-        <f>VLOOKUP(A29,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
-        <v>Cfx3-03</v>
-      </c>
-      <c r="C29">
-        <f>VLOOKUP(A29,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>989</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" t="str">
-        <f>VLOOKUP(A30,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
-        <v>Cfx3-03</v>
-      </c>
-      <c r="C30">
-        <f>VLOOKUP(A30,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" t="str">
-        <f>VLOOKUP(A31,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
-        <v>Cfx3-03</v>
-      </c>
-      <c r="C31">
-        <f>VLOOKUP(A31,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>833</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="str">
-        <f>VLOOKUP(A32,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,2,FALSE)</f>
-        <v>Cfx3-08</v>
-      </c>
-      <c r="C32">
-        <f>VLOOKUP(A32,'non-Chx-Geo-reads-S19.9-short'!$A$1:$C$45,3,FALSE)</f>
-        <v>346</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4">
-      <c r="C34">
-        <f>SUM(C29:C32)</f>
-        <v>3838</v>
-      </c>
-      <c r="D34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4">
-      <c r="C36">
-        <f>GETPIVOTDATA("reads",$A$3,"genome","Cfx3-03")-D3-C34</f>
-        <v>118523</v>
-      </c>
-      <c r="D36" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4">
-      <c r="C37" s="5">
-        <f>C36/GETPIVOTDATA("reads",$A$3,"genome","Cfx3-03")*100</f>
-        <v>96.860213296285707</v>
-      </c>
-      <c r="D37" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>